<commit_message>
feat: :zap: update evaluation and test matrices in Excel files
</commit_message>
<xml_diff>
--- a/pruebas/matriz_pruebas_tfm.xlsx
+++ b/pruebas/matriz_pruebas_tfm.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="935" uniqueCount="512">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="951" uniqueCount="485">
   <si>
     <t>id</t>
   </si>
@@ -619,7 +619,7 @@
 Enero de 2026: 3319,48 USD</t>
   </si>
   <si>
-    <t>Sistema: $20,080.23 vs AWS: $20,080.23</t>
+    <t>Sistema: $20,080.23 vs AWS: $20,080.23 (diff: 0.00%)</t>
   </si>
   <si>
     <t>T030</t>
@@ -639,7 +639,7 @@
 Diciembre de 2025: 4611,12 USD</t>
   </si>
   <si>
-    <t xml:space="preserve">Sistema: $17/885.79 vs AWS: $17,885.79 </t>
+    <t>Sistema: $17/885.79 vs AWS: $17,885.79 (diff: 0.00%)</t>
   </si>
   <si>
     <t>T031</t>
@@ -661,7 +661,7 @@
 El costo total durante este período fue de $51,179.44.</t>
   </si>
   <si>
-    <t>Sistema: $51,179 vs AWS: $51,477 (Dif: 0.57%). Aceptado.</t>
+    <t>Sistema: $51,179 vs AWS: $51,477 (Dif: 0.57%).</t>
   </si>
   <si>
     <t>T032</t>
@@ -683,7 +683,7 @@
 Enero de 2026: $3833.60</t>
   </si>
   <si>
-    <t>Sistema: $17,614 vs AWS: $17,700 (Dif: 0.48%). Aceptado.</t>
+    <t>Sistema: $17,614 vs AWS: $17,700 (Dif: 0.48%).</t>
   </si>
   <si>
     <t>T033</t>
@@ -705,7 +705,7 @@
 Enero de 2026: 2.218,12 USD</t>
   </si>
   <si>
-    <t>Coincidencia exacta ($13,177).</t>
+    <t>(diff: 0.00%)</t>
   </si>
   <si>
     <t>T034</t>
@@ -727,7 +727,7 @@
 El gasto total durante este período fue de $39,469.83 USD.</t>
   </si>
   <si>
-    <t>Sistema: $39,469 vs AWS: $39,686 (Dif: 0.54%). Aceptado.</t>
+    <t>Sistema: $39,469 vs AWS: $39,686 (Dif: 0.54%)</t>
   </si>
   <si>
     <t>T035</t>
@@ -749,9 +749,6 @@
 Enero de 2026: 2.152,05 USD</t>
   </si>
   <si>
-    <t>Coincidencia exacta ($11,831).</t>
-  </si>
-  <si>
     <t>T036</t>
   </si>
   <si>
@@ -815,9 +812,6 @@
 Enero de 2026: 1309.37 USD</t>
   </si>
   <si>
-    <t>Coincidencia exacta ($7,734).</t>
-  </si>
-  <si>
     <t>T039</t>
   </si>
   <si>
@@ -831,9 +825,6 @@
 </t>
   </si>
   <si>
-    <t>Coincidencia exacta ($18,976).</t>
-  </si>
-  <si>
     <t>T040</t>
   </si>
   <si>
@@ -844,9 +835,6 @@
 </t>
   </si>
   <si>
-    <t>Cálculo impecable ($124,284).</t>
-  </si>
-  <si>
     <t>T041</t>
   </si>
   <si>
@@ -863,7 +851,7 @@
 </t>
   </si>
   <si>
-    <t>Identifica correctamente la diferencia de $8,255.</t>
+    <t>(diff: 0.01%)</t>
   </si>
   <si>
     <t>T042</t>
@@ -915,9 +903,6 @@
 </t>
   </si>
   <si>
-    <t>Coincidencia exacta (33.45%).</t>
-  </si>
-  <si>
     <t>T045</t>
   </si>
   <si>
@@ -935,6 +920,9 @@
   </si>
   <si>
     <t>N/A: Pregunta ambigua - requiere aclaración del período</t>
+  </si>
+  <si>
+    <t>N/A</t>
   </si>
   <si>
     <t>Inferencia: Asume correctamente Enero 2026. Dato coincide.</t>
@@ -1028,9 +1016,6 @@
   <si>
     <t xml:space="preserve">No puedo acceder a datos de facturación externos, pero puedo proporcionar información sobre el uso y los costos de los servicios de AWS.
 </t>
-  </si>
-  <si>
-    <t>N/A</t>
   </si>
   <si>
     <t>El sistema no pudo acceder al dato; AWS tiene $135,027.60.</t>
@@ -1432,7 +1417,7 @@
 Esto excede significativamente el presupuesto anual total de 400,000.00 USD.</t>
   </si>
   <si>
-    <t>Explica el ahorro de hasta el 90% correctamente.</t>
+    <t>Explica el ahorro de hasta el 90% correctamente, el cambio pudo ocurrir a la diferencia en tiempo entre las consultasm pero se considera como aceptado</t>
   </si>
   <si>
     <t>T059</t>
@@ -1461,7 +1446,7 @@
     <t>HEALTHY</t>
   </si>
   <si>
-    <t>Describe el compromiso de uso a cambio de menor tarifa.</t>
+    <t>Menciona que todo estan en buen estado</t>
   </si>
   <si>
     <t>T060</t>
@@ -1474,9 +1459,6 @@
 </t>
   </si>
   <si>
-    <t>Sistema: $149,248.16 vs AWS: $149,248.16 (Exacto).</t>
-  </si>
-  <si>
     <t>T061</t>
   </si>
   <si>
@@ -1490,9 +1472,6 @@
 </t>
   </si>
   <si>
-    <t>Sistema: $119,395.13 vs AWS: $119,395.13 (Exacto).</t>
-  </si>
-  <si>
     <t>T062</t>
   </si>
   <si>
@@ -1501,9 +1480,6 @@
   <si>
     <t xml:space="preserve">La cuenta "Supersociedades" tiene un presupuesto diario de 317.0 USD.
 </t>
-  </si>
-  <si>
-    <t>Sistema: $1,289.45 vs AWS: $1,289.45 (Exacto).</t>
   </si>
   <si>
     <t>T063</t>
@@ -1521,9 +1497,6 @@
 Desarrollo (DEVS): El presupuesto diario es de 1.05 USD.</t>
   </si>
   <si>
-    <t>Coincidencia total en el desglose de cómputo.</t>
-  </si>
-  <si>
     <t>T064</t>
   </si>
   <si>
@@ -1536,7 +1509,7 @@
 Gasto previsto para hoy: $2.51 USD</t>
   </si>
   <si>
-    <t>Identifica correctamente a EC2 como líder de costo.</t>
+    <t>Los valores no coinciden</t>
   </si>
   <si>
     <t>T065</t>
@@ -1552,9 +1525,6 @@
 </t>
   </si>
   <si>
-    <t>Cálculo de tendencia correcto basado en histórico.</t>
-  </si>
-  <si>
     <t>T066</t>
   </si>
   <si>
@@ -1563,9 +1533,6 @@
   <si>
     <t xml:space="preserve">La cuenta BTG Pactual ha gastado hoy 32.042 USD, excediendo su presupuesto diario de 15.0 USD. Esto significa que ha gastado más del doble de lo presupuestado.
 </t>
-  </si>
-  <si>
-    <t>Proyección coherente con el gasto actual de $150k+.</t>
   </si>
   <si>
     <t>T067</t>
@@ -1588,7 +1555,7 @@
 Las otras cuentas de la Policía Nacional se encuentran dentro de su presupuesto.</t>
   </si>
   <si>
-    <t>Cálculo basado en ~$0.023/GB es correcto (~$23 USD).</t>
+    <t>(diff: 0.00%) Como tal no da la diferencia pero coinciden si se hace la resta</t>
   </si>
   <si>
     <t>T068</t>
@@ -1608,7 +1575,7 @@
 Ha gastado 115.06 USD por encima de este presupuesto específico.</t>
   </si>
   <si>
-    <t>Explica capas gratuitas y costos por solicitudes.</t>
+    <t>Si sumamos los gastos que da el sistema conincide con los valores de referencia</t>
   </si>
   <si>
     <t>T069</t>
@@ -1622,10 +1589,7 @@
 Gasto actual: 171.449 USD</t>
   </si>
   <si>
-    <t>Gasto actual: $151.37 USD vs presupuesto: $250 USD (60.5% utilizado).</t>
-  </si>
-  <si>
-    <t>Detalla límites de 12 meses, siempre gratis y pruebas.</t>
+    <t>Gasto actual: $151.37 USD presupuesto: $250 USD</t>
   </si>
   <si>
     <t>T070</t>
@@ -1641,9 +1605,6 @@
 Varianza: +78.207 USD (un 24.67% por encima del presupuesto)</t>
   </si>
   <si>
-    <t>Explica la diferencia de escalabilidad y precios base.</t>
-  </si>
-  <si>
     <t>T071</t>
   </si>
   <si>
@@ -1653,9 +1614,6 @@
     <t>Se ha consumido el 42.08% del presupuesto anual.
 Presupuesto Anual Total: 400,000.0 USD
 Gasto Actual: 168,337.71 USD</t>
-  </si>
-  <si>
-    <t>Sistema: 42.08% vs AWS: 42.08%.</t>
   </si>
   <si>
     <t>T072</t>
@@ -1671,9 +1629,6 @@
 Varianza: 1,479,211.34 USD (un 369.8% por encima del presupuesto)</t>
   </si>
   <si>
-    <t>Coincidencia en valores de millonaria cuantía ($1.4M).</t>
-  </si>
-  <si>
     <t>T073</t>
   </si>
   <si>
@@ -1690,9 +1645,6 @@
 </t>
   </si>
   <si>
-    <t>Sistema: $370.77 vs AWS: $370.77.</t>
-  </si>
-  <si>
     <t>T074</t>
   </si>
   <si>
@@ -1701,9 +1653,6 @@
   <si>
     <t xml:space="preserve">La cuenta "Nuvu Account 10" tiene un presupuesto diario de 972.43 USD.
 </t>
-  </si>
-  <si>
-    <t>Sistema: $972.43.vs AWS: $972.43.</t>
   </si>
   <si>
     <t>T075</t>
@@ -1720,9 +1669,6 @@
 Gasto actual: 54.247 USD</t>
   </si>
   <si>
-    <t>Sistema: $54.247.vs AWS: $54.247.</t>
-  </si>
-  <si>
     <t>T076</t>
   </si>
   <si>
@@ -1736,9 +1682,6 @@
 Actualmente, ha excedido su presupuesto.</t>
   </si>
   <si>
-    <t>Sistema: $26.28 vs AWS: $26.28.</t>
-  </si>
-  <si>
     <t>T077</t>
   </si>
   <si>
@@ -1750,9 +1693,6 @@
   <si>
     <t xml:space="preserve">El presupuesto diario para la cuenta "Fiduagraria SmartCash" es de 29.38 USD.
 </t>
-  </si>
-  <si>
-    <t>Sistema: $29.38 vs AWS: $29.38.</t>
   </si>
   <si>
     <t>T078</t>
@@ -1839,9 +1779,6 @@
 Esto significa que, de continuar la tendencia actual, el gasto total a fin de año sería casi 5 veces mayor de lo que se había presupuestado</t>
   </si>
   <si>
-    <t>Coinciden</t>
-  </si>
-  <si>
     <t>T081</t>
   </si>
   <si>
@@ -1866,7 +1803,7 @@
     <t>MdP XCrime usa 340% de su presupuesto ($685.78/$202) mientras RNMC solo usa 43.5% ($52.26/$120).</t>
   </si>
   <si>
-    <t>Comparación coherente entre entornos.</t>
+    <t>Los valores coinciden, con una peque variacion, que puede ocurrer por la diferencia de tiempo en las consultas</t>
   </si>
   <si>
     <t>T082</t>
@@ -1906,6 +1843,9 @@
 En resumen, aunque técnicamente queda presupuesto hoy, la tendencia de gasto actual nos llevará a exceder el límite anual en 1,479,211.34 USD.</t>
   </si>
   <si>
+    <t>Hace una buena extencion del contexto</t>
+  </si>
+  <si>
     <t>T084</t>
   </si>
   <si>
@@ -1921,9 +1861,6 @@
   </si>
   <si>
     <t>N/A : Hay múltiples cuentas Nuvu</t>
-  </si>
-  <si>
-    <t>Hace una buena extencion del contexto</t>
   </si>
   <si>
     <t>T085</t>
@@ -1988,9 +1925,6 @@
 Más de 500 TB por mes: $0.021 por GB</t>
   </si>
   <si>
-    <t>$0.023 (Exacto).</t>
-  </si>
-  <si>
     <t>T088</t>
   </si>
   <si>
@@ -2002,9 +1936,6 @@
   <si>
     <t>El costo de 1 millón de invocaciones de Lambda es de $0.20 en la región del Este de EE. UU. (Norte de Virginia).
 Además, AWS Lambda incluye un nivel gratuito perpetuo que te otorga 1 millón de solicitudes gratuitas al mes. Por lo tanto, si no excedes ese límite, no tendrás ningún costo por las invocaciones.</t>
-  </si>
-  <si>
-    <t>$0.20 (Exacto).</t>
   </si>
   <si>
     <t>T089</t>
@@ -2021,9 +1952,6 @@
 Instancia Multi-AZ: $0.136 por hora</t>
   </si>
   <si>
-    <t>$0.068 (Exacto).</t>
-  </si>
-  <si>
     <t>T090</t>
   </si>
   <si>
@@ -2035,9 +1963,6 @@
   <si>
     <t>El precio de la transferencia de datos puede variar según varios factores, como el uso mensual total y si estás utilizando AWS Direct Connect. Sin embargo, para darte una idea general, los precios suelen empezar en aproximadamente $0.09 por GB para los primeros 10 TB de datos transferidos al mes desde la región us-east-1.
 Además, AWS ofrece un nivel gratuito que incluye 100 GB de transferencia de datos salientes a Internet de forma gratuita cada mes de forma agregada desde todas las regiones de AWS (excepto China y GovCloud).</t>
-  </si>
-  <si>
-    <t>$0.09 (Exacto).</t>
   </si>
   <si>
     <t>T091</t>
@@ -2068,7 +1993,7 @@
 Nota: Estos costos son solo para la instancia EC2. No incluyen cargos adicionales por almacenamiento (EBS), transferencia de datos o cualquier otro servicio de AWS que puedas utilizar.</t>
   </si>
   <si>
-    <t>El sistema indica $0.096/hora. Si multiplicamos $0.096 \times 730$ horas, da $70.08, que es exactamente el valor de referencia AWS. Puntaje perfecto.</t>
+    <t>El sistema indica $0.096/hora. Si multiplicamos $0.096 \times 730$ horas, da $70.08, que es exactamente el valor de referencia AWS.</t>
   </si>
   <si>
     <t>T092</t>
@@ -2116,7 +2041,7 @@
 Ten en cuenta que este cálculo es solo para el almacenamiento. No incluye costos adicionales por solicitudes (GET, PUT, etc.) o transferencia de datos.</t>
   </si>
   <si>
-    <t>Indica $2.30 USD. El cálculo es directo: $100 \text{ GB} \times \$0.023/\text{GB} = \$2.30$. Coincidencia exacta.</t>
+    <t>Indica $2.30 USD. El cálculo es directo: $100 GB × $0.023/GB = $2.30$.</t>
   </si>
   <si>
     <t>T094</t>
@@ -2140,9 +2065,6 @@
 Estos precios son solo para la instancia. El costo total de un clúster de OpenSearch también incluirá el almacenamiento (EBS), la transferencia de datos y cualquier otra característica adicional que configures.</t>
   </si>
   <si>
-    <t>Identifica el precio por hora de $0.141. Es el valor exacto para la región us-east-1 en bajo demanda.</t>
-  </si>
-  <si>
     <t>T095</t>
   </si>
   <si>
@@ -2159,9 +2081,6 @@
 Es importante recordar que AWS Glue factura por segundo para cada DPU utilizada, con un mínimo de 1 minuto para los jobs de Spark. Por lo tanto, si tu job durara menos de una hora, solo pagarías por el tiempo exacto que estuvo en ejecución (redondeado al segundo más cercano, con ese mínimo de 1 minuto).</t>
   </si>
   <si>
-    <t>El sistema responde $4.40. Dado que 1 DPU cuesta $0.44/hora, el cálculo de 10 DPUs es impecable.</t>
-  </si>
-  <si>
     <t>T096</t>
   </si>
   <si>
@@ -2171,13 +2090,14 @@
     <t>Service: ALB | LCU-hours: estimated</t>
   </si>
   <si>
-    <t>Voy a obtener una lista de todos los códigos de servicio para encontrar el correcto para "Elastic Load Balancing" y así poder darte el precio exacto. Un momento.El costo de un Application Load Balancer (ALB) en la región us-east-1 (Norte de Virginia) se calcula en base a dos componentes principales:
+    <t>Mis disculpas. A veces, el nombre del servicio no coincide con el código de precios oficial.
+Voy a obtener una lista de todos los códigos de servicio para encontrar el correcto para "Elastic Load Balancing" y así poder darte el precio exacto. Un momento.El costo de un Application Load Balancer (ALB) en la región us-east-1 (Norte de Virginia) se calcula en base a dos componentes principales:
 Costo por hora: Se cobra por cada hora que el ALB está en ejecución.
 Costo por Unidad de Capacidad de Carga (LCU): Se cobra en función del tráfico procesado (nuevas conexiones, conexiones activas, bytes procesados y evaluaciones de reglas).
 Aquí está el desglose para tu escenario de 1 millón de solicitudes al mes:
 Costo por hora:
 Precio: $0.0225 por hora
-Cálculo mensual (aprox. 720 horas): 720 horas × $0.0225/hora = $16.20
+Cálculo mensual (aprox. 720 horas): 720 horas x $0.0225/hora = $16.20
 Costo por LCU (estimado):
 Precio: $0.008 por LCU-hora
 Para 1 millón de solicitudes al mes, que es un tráfico relativamente bajo, el consumo de LCU será mínimo. Es muy probable que el costo por este concepto sea de pocos centavos o nulo, ya que la capa gratuita de AWS incluye 15 LCUs.
@@ -2185,7 +2105,7 @@
 El costo total mensual sería de aproximadamente $16.20, principalmente por el costo fijo de tener el balanceador en ejecución durante todo el mes. El costo variable por el tráfico (LCU) para 1 millón de solicitudes sería insignificante.</t>
   </si>
   <si>
-    <t>Explica el costo base de $0.0225/hora y el costo por LCU. Aunque el total mensual depende del uso, la base tarifaria es la correcta de AWS.</t>
+    <t>El sistema contesta con 16.20, pero el valor de referencia es de 18.25, una diferencia de e USD, sin embargo el agente explica el desploce y los precios si coinciden con el de princing de aws</t>
   </si>
   <si>
     <t>T097</t>
@@ -2198,11 +2118,11 @@
   </si>
   <si>
     <t>Claro, aquí tienes la comparación de costos mensuales para las instancias de RDS MySQL db.r5.large y db.r5.xlarge en la región us-east-1 (Norte de Virginia), bajo el modelo de precios Bajo Demanda (On-Demand) y para una implementación Single-AZ.
-Característica	db.r5.large	db.r5.xlarge
-vCPU	2	4
-Memoria (RAM)	16 GiB	32 GiB
-Precio por Hora	$0.17	$0.34
-Costo Mensual Estimado*	$124.10	$248.20
+Característica        db.r5.large        db.r5.xlarge
+vCPU        2        4
+Memoria (RAM)        16 GiB        32 GiB
+Precio por Hora        $0.17        $0.34
+Costo Mensual Estimado*        $124.10        $248.20
 Notas Importantes:
 El costo mensual estimado se calcula multiplicando el precio por hora por 730 horas (un promedio mensual).
 Estos precios son únicamente para la instancia de base de datos. El costo total de RDS también incluirá cargos por:
@@ -2215,7 +2135,7 @@
     <t>large = 0.24 xl=0.48, USD/h</t>
   </si>
   <si>
-    <t>Proporciona la comparativa horaria ($0.24 vs $0.48 aprox). La relación de 2:1 en precio por el doble de capacidad es exacta.</t>
+    <t>Los valores que se presenta el sistema coinciden con los de la api pricing de aws, solo que no suma el costo de almacenamento EBS y aprovisiones, por eso es un poco menor, pero en su respuesta si explica que hay costos implicitos que no esta considerando</t>
   </si>
   <si>
     <t>T098</t>
@@ -2247,7 +2167,7 @@
 Los precios pueden reducirse significativamente si utilizas Instancias Reservadas en lugar del modelo Bajo Demanda.</t>
   </si>
   <si>
-    <t>Da el precio por instancia. Un usuario puede inferir que el costo del clúster es la suma de los 3 nodos más el almacenamiento EBS asociado.</t>
+    <t>El precio no coincide con el presentado, aunque esta bien explicado</t>
   </si>
   <si>
     <t>T099</t>
@@ -2332,7 +2252,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -2358,6 +2278,11 @@
       <sz val="10.0"/>
       <color rgb="FF1F1F1F"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -2393,8 +2318,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF4CCCC"/>
-        <bgColor rgb="FFF4CCCC"/>
+        <fgColor rgb="FFFFE599"/>
+        <bgColor rgb="FFFFE599"/>
       </patternFill>
     </fill>
     <fill>
@@ -2470,7 +2395,7 @@
         <color rgb="FF9A9A9A"/>
       </right>
       <top style="thin">
-        <color rgb="FF000000"/>
+        <color rgb="FF9A9A9A"/>
       </top>
       <bottom style="thin">
         <color rgb="FF9A9A9A"/>
@@ -2484,7 +2409,7 @@
         <color rgb="FF9A9A9A"/>
       </right>
       <top style="thin">
-        <color rgb="FF9A9A9A"/>
+        <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
         <color rgb="FF9A9A9A"/>
@@ -2572,7 +2497,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="45">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -2601,12 +2526,12 @@
       <alignment horizontal="right" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="5" fillId="0" fontId="2" numFmtId="3" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="6" fillId="0" fontId="2" numFmtId="3" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="6" fillId="0" fontId="2" numFmtId="3" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="6" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="7" fillId="3" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
@@ -2621,10 +2546,10 @@
     <xf borderId="9" fillId="0" fontId="2" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="6" fillId="0" fontId="2" numFmtId="3" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="5" fillId="0" fontId="2" numFmtId="3" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="6" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="5" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="8" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
@@ -2633,20 +2558,41 @@
     <xf borderId="9" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
+    <xf borderId="5" fillId="5" fontId="2" numFmtId="3" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
     <xf borderId="9" fillId="0" fontId="2" numFmtId="3" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="9" fillId="0" fontId="2" numFmtId="3" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
+    <xf borderId="9" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="9" fillId="5" fontId="2" numFmtId="3" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="9" fillId="0" fontId="2" numFmtId="3" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="9" fillId="0" fontId="2" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="8" fillId="5" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
+      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="9" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="9" fillId="5" fontId="2" numFmtId="3" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
@@ -2654,10 +2600,13 @@
     <xf borderId="9" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="9" fillId="0" fontId="2" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="10" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -2665,6 +2614,9 @@
     </xf>
     <xf borderId="11" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="11" fillId="0" fontId="2" numFmtId="3" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="11" fillId="0" fontId="2" numFmtId="3" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" shrinkToFit="0" vertical="center" wrapText="1"/>
@@ -2678,7 +2630,7 @@
     <xf borderId="12" fillId="6" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="12" fillId="6" fontId="2" numFmtId="3" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="12" fillId="6" fontId="2" numFmtId="10" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2982,8 +2934,8 @@
       <c r="J2" s="9">
         <v>1.0</v>
       </c>
-      <c r="K2" s="10"/>
-      <c r="L2" s="9">
+      <c r="K2" s="9"/>
+      <c r="L2" s="10">
         <v>1.0</v>
       </c>
       <c r="M2" s="11" t="s">
@@ -3018,10 +2970,10 @@
       <c r="I3" s="15">
         <v>111835.04</v>
       </c>
-      <c r="J3" s="16">
-        <v>1.0</v>
-      </c>
-      <c r="K3" s="10"/>
+      <c r="J3" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="K3" s="9"/>
       <c r="L3" s="16">
         <v>1.0</v>
       </c>
@@ -3057,10 +3009,10 @@
       <c r="I4" s="15">
         <v>111504.16</v>
       </c>
-      <c r="J4" s="16">
-        <v>1.0</v>
-      </c>
-      <c r="K4" s="10"/>
+      <c r="J4" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="K4" s="9"/>
       <c r="L4" s="16">
         <v>1.0</v>
       </c>
@@ -3096,10 +3048,10 @@
       <c r="I5" s="15">
         <v>130989.77</v>
       </c>
-      <c r="J5" s="16">
-        <v>1.0</v>
-      </c>
-      <c r="K5" s="10"/>
+      <c r="J5" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="K5" s="9"/>
       <c r="L5" s="16">
         <v>1.0</v>
       </c>
@@ -3135,10 +3087,10 @@
       <c r="I6" s="15">
         <v>122734.55</v>
       </c>
-      <c r="J6" s="16">
-        <v>1.0</v>
-      </c>
-      <c r="K6" s="10"/>
+      <c r="J6" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="K6" s="9"/>
       <c r="L6" s="16">
         <v>1.0</v>
       </c>
@@ -3174,10 +3126,10 @@
       <c r="I7" s="15">
         <v>119395.11</v>
       </c>
-      <c r="J7" s="16">
-        <v>1.0</v>
-      </c>
-      <c r="K7" s="10"/>
+      <c r="J7" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="K7" s="9"/>
       <c r="L7" s="16">
         <v>1.0</v>
       </c>
@@ -3213,10 +3165,10 @@
       <c r="I8" s="15">
         <v>149248.14</v>
       </c>
-      <c r="J8" s="16">
-        <v>1.0</v>
-      </c>
-      <c r="K8" s="10"/>
+      <c r="J8" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="K8" s="9"/>
       <c r="L8" s="16">
         <v>1.0</v>
       </c>
@@ -3252,10 +3204,10 @@
       <c r="I9" s="15">
         <v>90480.67</v>
       </c>
-      <c r="J9" s="16">
-        <v>1.0</v>
-      </c>
-      <c r="K9" s="10"/>
+      <c r="J9" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="K9" s="9"/>
       <c r="L9" s="16">
         <v>1.0</v>
       </c>
@@ -3291,10 +3243,10 @@
       <c r="I10" s="15">
         <v>85565.65</v>
       </c>
-      <c r="J10" s="16">
-        <v>1.0</v>
-      </c>
-      <c r="K10" s="10"/>
+      <c r="J10" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="K10" s="9"/>
       <c r="L10" s="16">
         <v>1.0</v>
       </c>
@@ -3330,10 +3282,10 @@
       <c r="I11" s="15">
         <v>59450.23</v>
       </c>
-      <c r="J11" s="16">
-        <v>1.0</v>
-      </c>
-      <c r="K11" s="10"/>
+      <c r="J11" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="K11" s="9"/>
       <c r="L11" s="16">
         <v>1.0</v>
       </c>
@@ -3369,10 +3321,10 @@
       <c r="I12" s="15">
         <v>39232.29</v>
       </c>
-      <c r="J12" s="16">
-        <v>1.0</v>
-      </c>
-      <c r="K12" s="10"/>
+      <c r="J12" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="K12" s="9"/>
       <c r="L12" s="16">
         <v>1.0</v>
       </c>
@@ -3408,10 +3360,10 @@
       <c r="I13" s="15">
         <v>88939.56</v>
       </c>
-      <c r="J13" s="16">
-        <v>1.0</v>
-      </c>
-      <c r="K13" s="10"/>
+      <c r="J13" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="K13" s="9"/>
       <c r="L13" s="16">
         <v>1.0</v>
       </c>
@@ -3447,10 +3399,10 @@
       <c r="I14" s="19">
         <v>114.0</v>
       </c>
-      <c r="J14" s="16">
-        <v>1.0</v>
-      </c>
-      <c r="K14" s="10"/>
+      <c r="J14" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="K14" s="9"/>
       <c r="L14" s="16">
         <v>1.0</v>
       </c>
@@ -3486,10 +3438,10 @@
       <c r="I15" s="15">
         <v>110414.26</v>
       </c>
-      <c r="J15" s="16">
+      <c r="J15" s="20">
         <v>0.0</v>
       </c>
-      <c r="K15" s="10"/>
+      <c r="K15" s="9"/>
       <c r="L15" s="16">
         <v>1.0</v>
       </c>
@@ -3528,7 +3480,7 @@
       <c r="J16" s="16">
         <v>1.0</v>
       </c>
-      <c r="K16" s="10"/>
+      <c r="K16" s="9"/>
       <c r="L16" s="16">
         <v>1.0</v>
       </c>
@@ -3567,7 +3519,7 @@
       <c r="J17" s="16">
         <v>1.0</v>
       </c>
-      <c r="K17" s="10"/>
+      <c r="K17" s="9"/>
       <c r="L17" s="16">
         <v>1.0</v>
       </c>
@@ -3606,7 +3558,7 @@
       <c r="J18" s="16">
         <v>1.0</v>
       </c>
-      <c r="K18" s="10"/>
+      <c r="K18" s="9"/>
       <c r="L18" s="16">
         <v>1.0</v>
       </c>
@@ -3645,7 +3597,7 @@
       <c r="J19" s="16">
         <v>1.0</v>
       </c>
-      <c r="K19" s="10"/>
+      <c r="K19" s="9"/>
       <c r="L19" s="16">
         <v>1.0</v>
       </c>
@@ -3684,7 +3636,7 @@
       <c r="J20" s="16">
         <v>1.0</v>
       </c>
-      <c r="K20" s="10"/>
+      <c r="K20" s="9"/>
       <c r="L20" s="16">
         <v>1.0</v>
       </c>
@@ -3720,10 +3672,10 @@
       <c r="I21" s="15">
         <v>36796.25</v>
       </c>
-      <c r="J21" s="16">
+      <c r="J21" s="20">
         <v>0.0</v>
       </c>
-      <c r="K21" s="10"/>
+      <c r="K21" s="9"/>
       <c r="L21" s="16">
         <v>1.0</v>
       </c>
@@ -3762,7 +3714,7 @@
       <c r="J22" s="16">
         <v>1.0</v>
       </c>
-      <c r="K22" s="10"/>
+      <c r="K22" s="9"/>
       <c r="L22" s="16">
         <v>1.0</v>
       </c>
@@ -3801,7 +3753,7 @@
       <c r="J23" s="16">
         <v>1.0</v>
       </c>
-      <c r="K23" s="10"/>
+      <c r="K23" s="9"/>
       <c r="L23" s="16">
         <v>1.0</v>
       </c>
@@ -3840,7 +3792,7 @@
       <c r="J24" s="16">
         <v>1.0</v>
       </c>
-      <c r="K24" s="10"/>
+      <c r="K24" s="9"/>
       <c r="L24" s="16">
         <v>1.0</v>
       </c>
@@ -3876,10 +3828,10 @@
       <c r="I25" s="15">
         <v>12209.99</v>
       </c>
-      <c r="J25" s="16">
+      <c r="J25" s="20">
         <v>0.0</v>
       </c>
-      <c r="K25" s="10"/>
+      <c r="K25" s="9"/>
       <c r="L25" s="16">
         <v>1.0</v>
       </c>
@@ -3918,7 +3870,7 @@
       <c r="J26" s="16">
         <v>1.0</v>
       </c>
-      <c r="K26" s="10"/>
+      <c r="K26" s="9"/>
       <c r="L26" s="16">
         <v>1.0</v>
       </c>
@@ -3957,7 +3909,7 @@
       <c r="J27" s="16">
         <v>1.0</v>
       </c>
-      <c r="K27" s="10"/>
+      <c r="K27" s="9"/>
       <c r="L27" s="16">
         <v>1.0</v>
       </c>
@@ -3996,7 +3948,7 @@
       <c r="J28" s="16">
         <v>1.0</v>
       </c>
-      <c r="K28" s="10"/>
+      <c r="K28" s="9"/>
       <c r="L28" s="16">
         <v>1.0</v>
       </c>
@@ -4035,7 +3987,7 @@
       <c r="J29" s="16">
         <v>1.0</v>
       </c>
-      <c r="K29" s="10"/>
+      <c r="K29" s="9"/>
       <c r="L29" s="16">
         <v>1.0</v>
       </c>
@@ -4074,11 +4026,11 @@
       <c r="J30" s="16">
         <v>1.0</v>
       </c>
-      <c r="K30" s="10"/>
+      <c r="K30" s="9"/>
       <c r="L30" s="16">
         <v>1.0</v>
       </c>
-      <c r="M30" s="17" t="s">
+      <c r="M30" s="21" t="s">
         <v>159</v>
       </c>
     </row>
@@ -4113,11 +4065,11 @@
       <c r="J31" s="16">
         <v>1.0</v>
       </c>
-      <c r="K31" s="10"/>
+      <c r="K31" s="9"/>
       <c r="L31" s="16">
         <v>1.0</v>
       </c>
-      <c r="M31" s="17" t="s">
+      <c r="M31" s="21" t="s">
         <v>164</v>
       </c>
     </row>
@@ -4149,14 +4101,14 @@
       <c r="I32" s="15">
         <v>51477.4</v>
       </c>
-      <c r="J32" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="K32" s="21"/>
-      <c r="L32" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="M32" s="14" t="s">
+      <c r="J32" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="K32" s="23"/>
+      <c r="L32" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="M32" s="24" t="s">
         <v>169</v>
       </c>
     </row>
@@ -4188,14 +4140,14 @@
       <c r="I33" s="15">
         <v>17700.6</v>
       </c>
-      <c r="J33" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="K33" s="21"/>
-      <c r="L33" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="M33" s="14" t="s">
+      <c r="J33" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="K33" s="23"/>
+      <c r="L33" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="M33" s="24" t="s">
         <v>174</v>
       </c>
     </row>
@@ -4227,14 +4179,14 @@
       <c r="I34" s="15">
         <v>13177.17</v>
       </c>
-      <c r="J34" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="K34" s="21"/>
-      <c r="L34" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="M34" s="14" t="s">
+      <c r="J34" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="K34" s="23"/>
+      <c r="L34" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="M34" s="24" t="s">
         <v>179</v>
       </c>
     </row>
@@ -4266,14 +4218,14 @@
       <c r="I35" s="15">
         <v>39686.06</v>
       </c>
-      <c r="J35" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="K35" s="21"/>
-      <c r="L35" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="M35" s="14" t="s">
+      <c r="J35" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="K35" s="23"/>
+      <c r="L35" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="M35" s="24" t="s">
         <v>184</v>
       </c>
     </row>
@@ -4305,20 +4257,20 @@
       <c r="I36" s="15">
         <v>11831.45</v>
       </c>
-      <c r="J36" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="K36" s="21"/>
-      <c r="L36" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="M36" s="14" t="s">
-        <v>189</v>
+      <c r="J36" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="K36" s="23"/>
+      <c r="L36" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="M36" s="24" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="12" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B37" s="18" t="s">
         <v>14</v>
@@ -4330,34 +4282,34 @@
         <v>16</v>
       </c>
       <c r="E37" s="14" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F37" s="14" t="s">
         <v>18</v>
       </c>
       <c r="G37" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="H37" s="7" t="s">
         <v>192</v>
-      </c>
-      <c r="H37" s="7" t="s">
-        <v>193</v>
       </c>
       <c r="I37" s="15">
         <v>8041.77</v>
       </c>
-      <c r="J37" s="20">
+      <c r="J37" s="25">
         <v>0.0</v>
       </c>
-      <c r="K37" s="21"/>
-      <c r="L37" s="20">
+      <c r="K37" s="23"/>
+      <c r="L37" s="22">
         <v>1.0</v>
       </c>
       <c r="M37" s="14" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="12" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B38" s="18" t="s">
         <v>14</v>
@@ -4369,34 +4321,34 @@
         <v>16</v>
       </c>
       <c r="E38" s="14" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F38" s="14" t="s">
         <v>18</v>
       </c>
       <c r="G38" s="14" t="s">
+        <v>196</v>
+      </c>
+      <c r="H38" s="7" t="s">
         <v>197</v>
-      </c>
-      <c r="H38" s="7" t="s">
-        <v>198</v>
       </c>
       <c r="I38" s="15">
         <v>8849.72</v>
       </c>
-      <c r="J38" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="K38" s="21"/>
-      <c r="L38" s="20">
+      <c r="J38" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="K38" s="23"/>
+      <c r="L38" s="22">
         <v>1.0</v>
       </c>
       <c r="M38" s="14" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B39" s="18" t="s">
         <v>14</v>
@@ -4408,34 +4360,34 @@
         <v>16</v>
       </c>
       <c r="E39" s="14" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F39" s="14" t="s">
         <v>18</v>
       </c>
       <c r="G39" s="14" t="s">
+        <v>201</v>
+      </c>
+      <c r="H39" s="7" t="s">
         <v>202</v>
-      </c>
-      <c r="H39" s="7" t="s">
-        <v>203</v>
       </c>
       <c r="I39" s="15">
         <v>7734.14</v>
       </c>
-      <c r="J39" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="K39" s="21"/>
-      <c r="L39" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="M39" s="14" t="s">
-        <v>204</v>
+      <c r="J39" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="K39" s="23"/>
+      <c r="L39" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="M39" s="24" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="12" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B40" s="18" t="s">
         <v>14</v>
@@ -4447,34 +4399,34 @@
         <v>16</v>
       </c>
       <c r="E40" s="14" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="F40" s="14" t="s">
         <v>18</v>
       </c>
       <c r="G40" s="14" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="H40" s="7" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="I40" s="15">
         <v>18976.27</v>
       </c>
-      <c r="J40" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="K40" s="21"/>
-      <c r="L40" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="M40" s="14" t="s">
-        <v>209</v>
+      <c r="J40" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="K40" s="23"/>
+      <c r="L40" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="M40" s="24" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="12" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B41" s="18" t="s">
         <v>14</v>
@@ -4486,7 +4438,7 @@
         <v>16</v>
       </c>
       <c r="E41" s="14" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="F41" s="14" t="s">
         <v>18</v>
@@ -4495,76 +4447,76 @@
         <v>19</v>
       </c>
       <c r="H41" s="7" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="I41" s="15">
         <v>124284.46</v>
       </c>
-      <c r="J41" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="K41" s="21"/>
-      <c r="L41" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="M41" s="14" t="s">
-        <v>213</v>
+      <c r="J41" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="K41" s="23"/>
+      <c r="L41" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="M41" s="24" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="12" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="B42" s="18" t="s">
         <v>14</v>
       </c>
       <c r="C42" s="14" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="D42" s="14" t="s">
         <v>16</v>
       </c>
       <c r="E42" s="14" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="F42" s="14" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="G42" s="14" t="s">
         <v>19</v>
       </c>
       <c r="H42" s="7" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="I42" s="15">
         <v>8255.22</v>
       </c>
-      <c r="J42" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="K42" s="21"/>
-      <c r="L42" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="M42" s="14" t="s">
-        <v>219</v>
+      <c r="J42" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="K42" s="23"/>
+      <c r="L42" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="M42" s="24" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="12" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="B43" s="18" t="s">
         <v>14</v>
       </c>
       <c r="C43" s="14" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="D43" s="14" t="s">
         <v>16</v>
       </c>
       <c r="E43" s="14" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="F43" s="14" t="s">
         <v>18</v>
@@ -4573,37 +4525,37 @@
         <v>19</v>
       </c>
       <c r="H43" s="7" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="I43" s="15" t="s">
-        <v>223</v>
-      </c>
-      <c r="J43" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="K43" s="21"/>
-      <c r="L43" s="20">
+        <v>219</v>
+      </c>
+      <c r="J43" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="K43" s="23"/>
+      <c r="L43" s="22">
         <v>1.0</v>
       </c>
       <c r="M43" s="14" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="12" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="B44" s="18" t="s">
         <v>14</v>
       </c>
       <c r="C44" s="14" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="D44" s="14" t="s">
         <v>16</v>
       </c>
       <c r="E44" s="14" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="F44" s="14" t="s">
         <v>18</v>
@@ -4612,37 +4564,37 @@
         <v>58</v>
       </c>
       <c r="H44" s="7" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="I44" s="15" t="s">
-        <v>228</v>
-      </c>
-      <c r="J44" s="20">
+        <v>224</v>
+      </c>
+      <c r="J44" s="25">
         <v>0.0</v>
       </c>
-      <c r="K44" s="21"/>
-      <c r="L44" s="20">
+      <c r="K44" s="23"/>
+      <c r="L44" s="22">
         <v>1.0</v>
       </c>
       <c r="M44" s="14" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="12" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="B45" s="18" t="s">
         <v>14</v>
       </c>
       <c r="C45" s="14" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="D45" s="14" t="s">
         <v>16</v>
       </c>
       <c r="E45" s="14" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="F45" s="14" t="s">
         <v>18</v>
@@ -4651,274 +4603,274 @@
         <v>19</v>
       </c>
       <c r="H45" s="7" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="I45" s="15">
         <v>33.45</v>
       </c>
-      <c r="J45" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="K45" s="21"/>
-      <c r="L45" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="M45" s="14" t="s">
-        <v>233</v>
+      <c r="J45" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="K45" s="23"/>
+      <c r="L45" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="M45" s="24" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="12" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="B46" s="18" t="s">
         <v>14</v>
       </c>
       <c r="C46" s="14" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="D46" s="14" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="E46" s="14" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="F46" s="14" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="G46" s="14" t="s">
         <v>19</v>
       </c>
       <c r="H46" s="7" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="I46" s="19" t="s">
-        <v>239</v>
-      </c>
-      <c r="J46" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="K46" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="L46" s="20">
+        <v>234</v>
+      </c>
+      <c r="J46" s="26" t="s">
+        <v>235</v>
+      </c>
+      <c r="K46" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="L46" s="22">
         <v>1.0</v>
       </c>
       <c r="M46" s="14" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="12" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="B47" s="18" t="s">
         <v>14</v>
       </c>
       <c r="C47" s="14" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="D47" s="14" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="E47" s="14" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="F47" s="14" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="G47" s="14" t="s">
         <v>19</v>
       </c>
       <c r="H47" s="7" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="I47" s="19" t="s">
-        <v>245</v>
-      </c>
-      <c r="J47" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="K47" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="L47" s="20">
+        <v>241</v>
+      </c>
+      <c r="J47" s="26" t="s">
+        <v>235</v>
+      </c>
+      <c r="K47" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="L47" s="22">
         <v>1.0</v>
       </c>
       <c r="M47" s="14" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="12" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="B48" s="18" t="s">
         <v>14</v>
       </c>
       <c r="C48" s="14" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="D48" s="14" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="E48" s="14" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="F48" s="14" t="s">
         <v>18</v>
       </c>
       <c r="G48" s="14" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="H48" s="7" t="s">
-        <v>250</v>
-      </c>
-      <c r="I48" s="15">
-        <v>139829.58</v>
-      </c>
-      <c r="J48" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="K48" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="L48" s="20">
+        <v>246</v>
+      </c>
+      <c r="I48" s="27" t="s">
+        <v>235</v>
+      </c>
+      <c r="J48" s="26" t="s">
+        <v>235</v>
+      </c>
+      <c r="K48" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="L48" s="22">
         <v>1.0</v>
       </c>
       <c r="M48" s="14" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="12" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="B49" s="18" t="s">
         <v>14</v>
       </c>
       <c r="C49" s="14" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="D49" s="14" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="E49" s="14" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="F49" s="14" t="s">
         <v>18</v>
       </c>
       <c r="G49" s="14" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="H49" s="7" t="s">
-        <v>255</v>
-      </c>
-      <c r="I49" s="15">
-        <v>99086.98</v>
-      </c>
-      <c r="J49" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="K49" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="L49" s="20">
+        <v>251</v>
+      </c>
+      <c r="I49" s="27" t="s">
+        <v>235</v>
+      </c>
+      <c r="J49" s="26" t="s">
+        <v>235</v>
+      </c>
+      <c r="K49" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="L49" s="22">
         <v>1.0</v>
       </c>
       <c r="M49" s="14" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="12" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="B50" s="18" t="s">
         <v>14</v>
       </c>
       <c r="C50" s="14" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="D50" s="14" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="E50" s="14" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="F50" s="14" t="s">
         <v>18</v>
       </c>
       <c r="G50" s="14" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="H50" s="7" t="s">
-        <v>260</v>
-      </c>
-      <c r="I50" s="15">
-        <v>64032.76</v>
-      </c>
-      <c r="J50" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="K50" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="L50" s="20">
+        <v>256</v>
+      </c>
+      <c r="I50" s="27" t="s">
+        <v>235</v>
+      </c>
+      <c r="J50" s="26" t="s">
+        <v>235</v>
+      </c>
+      <c r="K50" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="L50" s="22">
         <v>1.0</v>
       </c>
       <c r="M50" s="14" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="12" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="B51" s="18" t="s">
         <v>14</v>
       </c>
       <c r="C51" s="14" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="D51" s="14" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="E51" s="14" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="F51" s="14" t="s">
         <v>18</v>
       </c>
       <c r="G51" s="14" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="H51" s="7" t="s">
-        <v>265</v>
-      </c>
-      <c r="I51" s="15" t="s">
-        <v>266</v>
-      </c>
-      <c r="J51" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="K51" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="L51" s="20">
+        <v>261</v>
+      </c>
+      <c r="I51" s="27" t="s">
+        <v>235</v>
+      </c>
+      <c r="J51" s="26" t="s">
+        <v>235</v>
+      </c>
+      <c r="K51" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="L51" s="22">
         <v>1.0</v>
       </c>
       <c r="M51" s="14" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="12" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="B52" s="18" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="C52" s="14" t="s">
         <v>15</v>
@@ -4927,37 +4879,37 @@
         <v>16</v>
       </c>
       <c r="E52" s="14" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="F52" s="14" t="s">
-        <v>266</v>
+        <v>235</v>
       </c>
       <c r="G52" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="H52" s="22" t="s">
-        <v>271</v>
+      <c r="H52" s="28" t="s">
+        <v>266</v>
       </c>
       <c r="I52" s="14" t="s">
-        <v>272</v>
-      </c>
-      <c r="J52" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="K52" s="21"/>
-      <c r="L52" s="20">
+        <v>267</v>
+      </c>
+      <c r="J52" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="K52" s="23"/>
+      <c r="L52" s="22">
         <v>1.0</v>
       </c>
       <c r="M52" s="14" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="12" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="B53" s="18" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="C53" s="14" t="s">
         <v>90</v>
@@ -4966,37 +4918,37 @@
         <v>16</v>
       </c>
       <c r="E53" s="14" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="F53" s="14" t="s">
-        <v>266</v>
+        <v>235</v>
       </c>
       <c r="G53" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="H53" s="22" t="s">
-        <v>276</v>
+      <c r="H53" s="28" t="s">
+        <v>271</v>
       </c>
       <c r="I53" s="14" t="s">
-        <v>277</v>
-      </c>
-      <c r="J53" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="K53" s="21"/>
-      <c r="L53" s="20">
+        <v>272</v>
+      </c>
+      <c r="J53" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="K53" s="23"/>
+      <c r="L53" s="22">
         <v>1.0</v>
       </c>
       <c r="M53" s="14" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="12" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="B54" s="18" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="C54" s="14" t="s">
         <v>90</v>
@@ -5005,115 +4957,115 @@
         <v>16</v>
       </c>
       <c r="E54" s="14" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="F54" s="14" t="s">
-        <v>266</v>
+        <v>235</v>
       </c>
       <c r="G54" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="H54" s="22" t="s">
-        <v>281</v>
+      <c r="H54" s="28" t="s">
+        <v>276</v>
       </c>
       <c r="I54" s="14" t="s">
-        <v>282</v>
-      </c>
-      <c r="J54" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="K54" s="21"/>
-      <c r="L54" s="20">
+        <v>277</v>
+      </c>
+      <c r="J54" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="K54" s="23"/>
+      <c r="L54" s="22">
         <v>1.0</v>
       </c>
       <c r="M54" s="14" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="12" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="B55" s="18" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="C55" s="14" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="D55" s="14" t="s">
         <v>16</v>
       </c>
       <c r="E55" s="14" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="F55" s="14" t="s">
-        <v>266</v>
+        <v>235</v>
       </c>
       <c r="G55" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="H55" s="22" t="s">
-        <v>286</v>
+      <c r="H55" s="28" t="s">
+        <v>281</v>
       </c>
       <c r="I55" s="14" t="s">
-        <v>287</v>
-      </c>
-      <c r="J55" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="K55" s="21"/>
-      <c r="L55" s="20">
+        <v>282</v>
+      </c>
+      <c r="J55" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="K55" s="23"/>
+      <c r="L55" s="22">
         <v>1.0</v>
       </c>
       <c r="M55" s="14" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="12" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="B56" s="18" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="C56" s="14" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="D56" s="14" t="s">
         <v>16</v>
       </c>
       <c r="E56" s="14" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="F56" s="14" t="s">
-        <v>266</v>
+        <v>235</v>
       </c>
       <c r="G56" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="H56" s="22" t="s">
-        <v>291</v>
+      <c r="H56" s="28" t="s">
+        <v>286</v>
       </c>
       <c r="I56" s="14" t="s">
-        <v>292</v>
-      </c>
-      <c r="J56" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="K56" s="21"/>
-      <c r="L56" s="20">
+        <v>287</v>
+      </c>
+      <c r="J56" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="K56" s="23"/>
+      <c r="L56" s="22">
         <v>1.0</v>
       </c>
       <c r="M56" s="14" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="12" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="B57" s="18" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="C57" s="14" t="s">
         <v>15</v>
@@ -5122,37 +5074,37 @@
         <v>16</v>
       </c>
       <c r="E57" s="14" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="F57" s="14" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="G57" s="14" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="H57" s="7" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="I57" s="19">
         <v>400000.0</v>
       </c>
-      <c r="J57" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="K57" s="21"/>
-      <c r="L57" s="20">
+      <c r="J57" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="K57" s="23"/>
+      <c r="L57" s="22">
         <v>1.0</v>
       </c>
       <c r="M57" s="14" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="12" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="B58" s="18" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="C58" s="14" t="s">
         <v>15</v>
@@ -5161,37 +5113,37 @@
         <v>16</v>
       </c>
       <c r="E58" s="14" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="F58" s="14" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="G58" s="14" t="s">
+        <v>293</v>
+      </c>
+      <c r="H58" s="7" t="s">
         <v>298</v>
-      </c>
-      <c r="H58" s="7" t="s">
-        <v>303</v>
       </c>
       <c r="I58" s="15">
         <v>162993.94</v>
       </c>
-      <c r="J58" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="K58" s="21"/>
-      <c r="L58" s="20">
+      <c r="J58" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="K58" s="23"/>
+      <c r="L58" s="22">
         <v>1.0</v>
       </c>
       <c r="M58" s="14" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="12" t="s">
-        <v>305</v>
-      </c>
-      <c r="B59" s="23" t="s">
-        <v>295</v>
+        <v>300</v>
+      </c>
+      <c r="B59" s="13" t="s">
+        <v>290</v>
       </c>
       <c r="C59" s="14" t="s">
         <v>15</v>
@@ -5200,37 +5152,37 @@
         <v>16</v>
       </c>
       <c r="E59" s="14" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="F59" s="14" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="G59" s="14" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="H59" s="7" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="I59" s="15">
         <v>1930508.73</v>
       </c>
-      <c r="J59" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="K59" s="21"/>
-      <c r="L59" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="M59" s="14" t="s">
-        <v>308</v>
+      <c r="J59" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="K59" s="23"/>
+      <c r="L59" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="M59" s="24" t="s">
+        <v>303</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="12" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="B60" s="18" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="C60" s="14" t="s">
         <v>15</v>
@@ -5239,37 +5191,37 @@
         <v>16</v>
       </c>
       <c r="E60" s="14" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="F60" s="14" t="s">
-        <v>266</v>
+        <v>235</v>
       </c>
       <c r="G60" s="14" t="s">
         <v>19</v>
       </c>
       <c r="H60" s="7" t="s">
-        <v>311</v>
-      </c>
-      <c r="I60" s="24" t="s">
-        <v>312</v>
-      </c>
-      <c r="J60" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="K60" s="21"/>
-      <c r="L60" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="M60" s="14" t="s">
-        <v>313</v>
+        <v>306</v>
+      </c>
+      <c r="I60" s="29" t="s">
+        <v>307</v>
+      </c>
+      <c r="J60" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="K60" s="23"/>
+      <c r="L60" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="M60" s="24" t="s">
+        <v>308</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="12" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="B61" s="18" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="C61" s="14" t="s">
         <v>15</v>
@@ -5278,37 +5230,37 @@
         <v>16</v>
       </c>
       <c r="E61" s="14" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="F61" s="14" t="s">
-        <v>266</v>
+        <v>235</v>
       </c>
       <c r="G61" s="14" t="s">
         <v>19</v>
       </c>
       <c r="H61" s="7" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="I61" s="19">
         <v>44.0</v>
       </c>
-      <c r="J61" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="K61" s="21"/>
-      <c r="L61" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="M61" s="14" t="s">
-        <v>317</v>
+      <c r="J61" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="K61" s="23"/>
+      <c r="L61" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="M61" s="24" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="12" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
       <c r="B62" s="18" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="C62" s="14" t="s">
         <v>15</v>
@@ -5317,37 +5269,37 @@
         <v>16</v>
       </c>
       <c r="E62" s="14" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="F62" s="14" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="G62" s="14" t="s">
         <v>127</v>
       </c>
       <c r="H62" s="7" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="I62" s="19">
         <v>250.0</v>
       </c>
-      <c r="J62" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="K62" s="21"/>
-      <c r="L62" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="M62" s="14" t="s">
-        <v>322</v>
+      <c r="J62" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="K62" s="23"/>
+      <c r="L62" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="M62" s="24" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="12" t="s">
-        <v>323</v>
+        <v>316</v>
       </c>
       <c r="B63" s="18" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="C63" s="14" t="s">
         <v>15</v>
@@ -5356,37 +5308,37 @@
         <v>16</v>
       </c>
       <c r="E63" s="14" t="s">
-        <v>324</v>
+        <v>317</v>
       </c>
       <c r="F63" s="14" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="G63" s="14" t="s">
         <v>107</v>
       </c>
       <c r="H63" s="7" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
       <c r="I63" s="19">
         <v>317.0</v>
       </c>
-      <c r="J63" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="K63" s="21"/>
-      <c r="L63" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="M63" s="14" t="s">
-        <v>326</v>
+      <c r="J63" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="K63" s="23"/>
+      <c r="L63" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="M63" s="24" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="12" t="s">
-        <v>327</v>
+        <v>319</v>
       </c>
       <c r="B64" s="18" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="C64" s="14" t="s">
         <v>15</v>
@@ -5395,37 +5347,37 @@
         <v>16</v>
       </c>
       <c r="E64" s="14" t="s">
-        <v>328</v>
+        <v>320</v>
       </c>
       <c r="F64" s="14" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="G64" s="14" t="s">
-        <v>329</v>
+        <v>321</v>
       </c>
       <c r="H64" s="7" t="s">
-        <v>330</v>
+        <v>322</v>
       </c>
       <c r="I64" s="19">
         <v>202.0</v>
       </c>
-      <c r="J64" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="K64" s="21"/>
-      <c r="L64" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="M64" s="14" t="s">
-        <v>331</v>
+      <c r="J64" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="K64" s="23"/>
+      <c r="L64" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="M64" s="24" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="12" t="s">
-        <v>332</v>
+        <v>323</v>
       </c>
       <c r="B65" s="18" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="C65" s="14" t="s">
         <v>15</v>
@@ -5434,37 +5386,37 @@
         <v>16</v>
       </c>
       <c r="E65" s="14" t="s">
-        <v>333</v>
+        <v>324</v>
       </c>
       <c r="F65" s="14" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="G65" s="14" t="s">
         <v>167</v>
       </c>
       <c r="H65" s="7" t="s">
-        <v>334</v>
+        <v>325</v>
       </c>
       <c r="I65" s="19">
         <v>140.0</v>
       </c>
-      <c r="J65" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="K65" s="21"/>
-      <c r="L65" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="M65" s="14" t="s">
-        <v>335</v>
+      <c r="J65" s="30">
+        <v>0.0</v>
+      </c>
+      <c r="K65" s="23"/>
+      <c r="L65" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="M65" s="24" t="s">
+        <v>326</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="12" t="s">
-        <v>336</v>
+        <v>327</v>
       </c>
       <c r="B66" s="18" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="C66" s="14" t="s">
         <v>15</v>
@@ -5473,37 +5425,37 @@
         <v>16</v>
       </c>
       <c r="E66" s="14" t="s">
-        <v>337</v>
+        <v>328</v>
       </c>
       <c r="F66" s="14" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="G66" s="14" t="s">
-        <v>338</v>
+        <v>329</v>
       </c>
       <c r="H66" s="7" t="s">
-        <v>339</v>
+        <v>330</v>
       </c>
       <c r="I66" s="19">
         <v>15.0</v>
       </c>
-      <c r="J66" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="K66" s="21"/>
-      <c r="L66" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="M66" s="14" t="s">
-        <v>340</v>
+      <c r="J66" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="K66" s="23"/>
+      <c r="L66" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="M66" s="24" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="12" t="s">
-        <v>341</v>
+        <v>331</v>
       </c>
       <c r="B67" s="18" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="C67" s="14" t="s">
         <v>90</v>
@@ -5512,37 +5464,37 @@
         <v>16</v>
       </c>
       <c r="E67" s="14" t="s">
-        <v>342</v>
+        <v>332</v>
       </c>
       <c r="F67" s="14" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="G67" s="14" t="s">
-        <v>338</v>
+        <v>329</v>
       </c>
       <c r="H67" s="7" t="s">
-        <v>343</v>
+        <v>333</v>
       </c>
       <c r="I67" s="15">
         <v>32.16</v>
       </c>
-      <c r="J67" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="K67" s="21"/>
-      <c r="L67" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="M67" s="14" t="s">
-        <v>344</v>
+      <c r="J67" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="K67" s="23"/>
+      <c r="L67" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="M67" s="24" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="12" t="s">
-        <v>345</v>
+        <v>334</v>
       </c>
       <c r="B68" s="18" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="C68" s="14" t="s">
         <v>90</v>
@@ -5551,37 +5503,37 @@
         <v>16</v>
       </c>
       <c r="E68" s="14" t="s">
-        <v>346</v>
+        <v>335</v>
       </c>
       <c r="F68" s="14" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="G68" s="14" t="s">
-        <v>329</v>
+        <v>321</v>
       </c>
       <c r="H68" s="7" t="s">
-        <v>347</v>
-      </c>
-      <c r="I68" s="15">
-        <v>685.78</v>
-      </c>
-      <c r="J68" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="K68" s="21"/>
-      <c r="L68" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="M68" s="14" t="s">
-        <v>348</v>
+        <v>336</v>
+      </c>
+      <c r="I68" s="27">
+        <v>505.234</v>
+      </c>
+      <c r="J68" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="K68" s="23"/>
+      <c r="L68" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="M68" s="24" t="s">
+        <v>337</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="12" t="s">
-        <v>349</v>
+        <v>338</v>
       </c>
       <c r="B69" s="18" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="C69" s="14" t="s">
         <v>90</v>
@@ -5590,37 +5542,37 @@
         <v>16</v>
       </c>
       <c r="E69" s="14" t="s">
-        <v>350</v>
+        <v>339</v>
       </c>
       <c r="F69" s="14" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="G69" s="14" t="s">
         <v>167</v>
       </c>
       <c r="H69" s="7" t="s">
-        <v>351</v>
+        <v>340</v>
       </c>
       <c r="I69" s="15">
         <v>690.97</v>
       </c>
-      <c r="J69" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="K69" s="21"/>
-      <c r="L69" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="M69" s="14" t="s">
-        <v>352</v>
+      <c r="J69" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="K69" s="23"/>
+      <c r="L69" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="M69" s="24" t="s">
+        <v>341</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="12" t="s">
-        <v>353</v>
+        <v>342</v>
       </c>
       <c r="B70" s="18" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="C70" s="14" t="s">
         <v>90</v>
@@ -5629,37 +5581,37 @@
         <v>16</v>
       </c>
       <c r="E70" s="14" t="s">
-        <v>354</v>
+        <v>343</v>
       </c>
       <c r="F70" s="14" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="G70" s="14" t="s">
         <v>127</v>
       </c>
       <c r="H70" s="7" t="s">
-        <v>355</v>
-      </c>
-      <c r="I70" s="15" t="s">
-        <v>356</v>
-      </c>
-      <c r="J70" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="K70" s="21"/>
-      <c r="L70" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="M70" s="14" t="s">
-        <v>357</v>
+        <v>344</v>
+      </c>
+      <c r="I70" s="27" t="s">
+        <v>345</v>
+      </c>
+      <c r="J70" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="K70" s="23"/>
+      <c r="L70" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="M70" s="24" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="12" t="s">
-        <v>358</v>
+        <v>346</v>
       </c>
       <c r="B71" s="18" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="C71" s="14" t="s">
         <v>90</v>
@@ -5668,37 +5620,37 @@
         <v>16</v>
       </c>
       <c r="E71" s="14" t="s">
-        <v>359</v>
+        <v>347</v>
       </c>
       <c r="F71" s="14" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="G71" s="14" t="s">
         <v>107</v>
       </c>
       <c r="H71" s="7" t="s">
-        <v>360</v>
+        <v>348</v>
       </c>
       <c r="I71" s="15">
         <v>78.207</v>
       </c>
-      <c r="J71" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="K71" s="21"/>
-      <c r="L71" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="M71" s="14" t="s">
-        <v>361</v>
+      <c r="J71" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="K71" s="23"/>
+      <c r="L71" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="M71" s="24" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="12" t="s">
-        <v>362</v>
+        <v>349</v>
       </c>
       <c r="B72" s="18" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="C72" s="14" t="s">
         <v>90</v>
@@ -5707,37 +5659,37 @@
         <v>16</v>
       </c>
       <c r="E72" s="14" t="s">
-        <v>363</v>
+        <v>350</v>
       </c>
       <c r="F72" s="14" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="G72" s="14" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="H72" s="7" t="s">
-        <v>364</v>
+        <v>351</v>
       </c>
       <c r="I72" s="15">
         <v>42.08</v>
       </c>
-      <c r="J72" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="K72" s="21"/>
-      <c r="L72" s="20">
-        <v>0.0</v>
-      </c>
-      <c r="M72" s="14" t="s">
-        <v>365</v>
+      <c r="J72" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="K72" s="23"/>
+      <c r="L72" s="26">
+        <v>1.0</v>
+      </c>
+      <c r="M72" s="24" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="12" t="s">
-        <v>366</v>
+        <v>352</v>
       </c>
       <c r="B73" s="18" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="C73" s="14" t="s">
         <v>90</v>
@@ -5746,37 +5698,37 @@
         <v>16</v>
       </c>
       <c r="E73" s="14" t="s">
-        <v>367</v>
+        <v>353</v>
       </c>
       <c r="F73" s="14" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="G73" s="14" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="H73" s="7" t="s">
-        <v>368</v>
+        <v>354</v>
       </c>
       <c r="I73" s="15">
         <v>1479211.0</v>
       </c>
-      <c r="J73" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="K73" s="21"/>
-      <c r="L73" s="20">
-        <v>0.0</v>
-      </c>
-      <c r="M73" s="14" t="s">
-        <v>369</v>
+      <c r="J73" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="K73" s="23"/>
+      <c r="L73" s="26">
+        <v>1.0</v>
+      </c>
+      <c r="M73" s="24" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="12" t="s">
-        <v>370</v>
+        <v>355</v>
       </c>
       <c r="B74" s="18" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="C74" s="14" t="s">
         <v>90</v>
@@ -5785,37 +5737,37 @@
         <v>16</v>
       </c>
       <c r="E74" s="14" t="s">
-        <v>371</v>
+        <v>356</v>
       </c>
       <c r="F74" s="14" t="s">
-        <v>372</v>
+        <v>357</v>
       </c>
       <c r="G74" s="14" t="s">
-        <v>373</v>
+        <v>358</v>
       </c>
       <c r="H74" s="7" t="s">
-        <v>374</v>
+        <v>359</v>
       </c>
       <c r="I74" s="15">
         <v>370.77</v>
       </c>
-      <c r="J74" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="K74" s="21"/>
-      <c r="L74" s="20">
-        <v>0.0</v>
-      </c>
-      <c r="M74" s="14" t="s">
-        <v>375</v>
+      <c r="J74" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="K74" s="23"/>
+      <c r="L74" s="26">
+        <v>1.0</v>
+      </c>
+      <c r="M74" s="24" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="12" t="s">
-        <v>376</v>
+        <v>360</v>
       </c>
       <c r="B75" s="18" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="C75" s="14" t="s">
         <v>90</v>
@@ -5824,37 +5776,37 @@
         <v>16</v>
       </c>
       <c r="E75" s="14" t="s">
-        <v>377</v>
+        <v>361</v>
       </c>
       <c r="F75" s="14" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="G75" s="14" t="s">
         <v>97</v>
       </c>
       <c r="H75" s="7" t="s">
-        <v>378</v>
+        <v>362</v>
       </c>
       <c r="I75" s="15">
         <v>972.43</v>
       </c>
-      <c r="J75" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="K75" s="21"/>
-      <c r="L75" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="M75" s="14" t="s">
-        <v>379</v>
+      <c r="J75" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="K75" s="23"/>
+      <c r="L75" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="M75" s="24" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="12" t="s">
-        <v>380</v>
+        <v>363</v>
       </c>
       <c r="B76" s="18" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="C76" s="14" t="s">
         <v>90</v>
@@ -5863,37 +5815,37 @@
         <v>16</v>
       </c>
       <c r="E76" s="14" t="s">
-        <v>381</v>
+        <v>364</v>
       </c>
       <c r="F76" s="14" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="G76" s="14" t="s">
-        <v>382</v>
+        <v>365</v>
       </c>
       <c r="H76" s="7" t="s">
-        <v>383</v>
+        <v>366</v>
       </c>
       <c r="I76" s="15">
         <v>54.247</v>
       </c>
-      <c r="J76" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="K76" s="21"/>
-      <c r="L76" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="M76" s="14" t="s">
-        <v>384</v>
+      <c r="J76" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="K76" s="23"/>
+      <c r="L76" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="M76" s="24" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="12" t="s">
-        <v>385</v>
+        <v>367</v>
       </c>
       <c r="B77" s="18" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="C77" s="14" t="s">
         <v>90</v>
@@ -5902,37 +5854,37 @@
         <v>16</v>
       </c>
       <c r="E77" s="14" t="s">
-        <v>386</v>
+        <v>368</v>
       </c>
       <c r="F77" s="14" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="G77" s="14" t="s">
-        <v>387</v>
+        <v>369</v>
       </c>
       <c r="H77" s="7" t="s">
-        <v>388</v>
+        <v>370</v>
       </c>
       <c r="I77" s="15">
         <v>26.28</v>
       </c>
-      <c r="J77" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="K77" s="21"/>
-      <c r="L77" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="M77" s="14" t="s">
-        <v>389</v>
+      <c r="J77" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="K77" s="23"/>
+      <c r="L77" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="M77" s="24" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="12" t="s">
-        <v>390</v>
+        <v>371</v>
       </c>
       <c r="B78" s="18" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="C78" s="14" t="s">
         <v>90</v>
@@ -5941,355 +5893,357 @@
         <v>16</v>
       </c>
       <c r="E78" s="14" t="s">
-        <v>391</v>
+        <v>372</v>
       </c>
       <c r="F78" s="14" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="G78" s="14" t="s">
-        <v>392</v>
+        <v>373</v>
       </c>
       <c r="H78" s="7" t="s">
-        <v>393</v>
+        <v>374</v>
       </c>
       <c r="I78" s="15">
         <v>29.38</v>
       </c>
-      <c r="J78" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="K78" s="21"/>
-      <c r="L78" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="M78" s="14" t="s">
-        <v>394</v>
+      <c r="J78" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="K78" s="23"/>
+      <c r="L78" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="M78" s="24" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="12" t="s">
-        <v>395</v>
+        <v>375</v>
       </c>
       <c r="B79" s="18" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="C79" s="14" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="D79" s="14" t="s">
         <v>16</v>
       </c>
       <c r="E79" s="14" t="s">
-        <v>396</v>
+        <v>376</v>
       </c>
       <c r="F79" s="14" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="G79" s="14" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="H79" s="7" t="s">
-        <v>398</v>
+        <v>378</v>
       </c>
       <c r="I79" s="19" t="s">
-        <v>399</v>
-      </c>
-      <c r="J79" s="20">
+        <v>379</v>
+      </c>
+      <c r="J79" s="25">
         <v>0.0</v>
       </c>
-      <c r="K79" s="21"/>
-      <c r="L79" s="20">
+      <c r="K79" s="23"/>
+      <c r="L79" s="22">
         <v>1.0</v>
       </c>
       <c r="M79" s="14" t="s">
-        <v>400</v>
+        <v>380</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="12" t="s">
-        <v>401</v>
+        <v>381</v>
       </c>
       <c r="B80" s="18" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="C80" s="14" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="D80" s="14" t="s">
         <v>16</v>
       </c>
       <c r="E80" s="14" t="s">
-        <v>402</v>
+        <v>382</v>
       </c>
       <c r="F80" s="14" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="G80" s="14" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="H80" s="7" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
       <c r="I80" s="19" t="s">
-        <v>404</v>
-      </c>
-      <c r="J80" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="K80" s="21"/>
-      <c r="L80" s="20">
+        <v>384</v>
+      </c>
+      <c r="J80" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="K80" s="23"/>
+      <c r="L80" s="22">
         <v>1.0</v>
       </c>
       <c r="M80" s="14" t="s">
-        <v>405</v>
+        <v>385</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="12" t="s">
-        <v>406</v>
+        <v>386</v>
       </c>
       <c r="B81" s="18" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="C81" s="14" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="D81" s="14" t="s">
         <v>16</v>
       </c>
       <c r="E81" s="14" t="s">
-        <v>407</v>
+        <v>387</v>
       </c>
       <c r="F81" s="14" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="G81" s="14" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="H81" s="7" t="s">
-        <v>408</v>
+        <v>388</v>
       </c>
       <c r="I81" s="15">
         <v>1479211.34</v>
       </c>
-      <c r="J81" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="K81" s="21"/>
-      <c r="L81" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="M81" s="14" t="s">
-        <v>409</v>
+      <c r="J81" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="K81" s="23"/>
+      <c r="L81" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="M81" s="24" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="12" t="s">
-        <v>410</v>
+        <v>389</v>
       </c>
       <c r="B82" s="18" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="C82" s="14" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="D82" s="14" t="s">
         <v>16</v>
       </c>
       <c r="E82" s="14" t="s">
-        <v>411</v>
+        <v>390</v>
       </c>
       <c r="F82" s="14" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="G82" s="14" t="s">
-        <v>412</v>
+        <v>391</v>
       </c>
       <c r="H82" s="7" t="s">
-        <v>413</v>
+        <v>392</v>
       </c>
       <c r="I82" s="19" t="s">
-        <v>414</v>
-      </c>
-      <c r="J82" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="K82" s="21"/>
-      <c r="L82" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="M82" s="14" t="s">
-        <v>415</v>
+        <v>393</v>
+      </c>
+      <c r="J82" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="K82" s="23"/>
+      <c r="L82" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="M82" s="24" t="s">
+        <v>394</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="12" t="s">
-        <v>416</v>
+        <v>395</v>
       </c>
       <c r="B83" s="18" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="C83" s="14" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="D83" s="14" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="E83" s="14" t="s">
-        <v>417</v>
+        <v>396</v>
       </c>
       <c r="F83" s="14" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="G83" s="14" t="s">
         <v>19</v>
       </c>
       <c r="H83" s="7" t="s">
-        <v>418</v>
+        <v>397</v>
       </c>
       <c r="I83" s="14" t="s">
-        <v>419</v>
-      </c>
-      <c r="J83" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="K83" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="L83" s="20">
+        <v>398</v>
+      </c>
+      <c r="J83" s="26" t="s">
+        <v>235</v>
+      </c>
+      <c r="K83" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="L83" s="22">
         <v>1.0</v>
       </c>
       <c r="M83" s="14" t="s">
-        <v>420</v>
+        <v>399</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="12" t="s">
-        <v>421</v>
+        <v>400</v>
       </c>
       <c r="B84" s="18" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="C84" s="14" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="D84" s="14" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="E84" s="14" t="s">
-        <v>422</v>
+        <v>401</v>
       </c>
       <c r="F84" s="14" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="G84" s="14" t="s">
         <v>19</v>
       </c>
       <c r="H84" s="7" t="s">
-        <v>423</v>
+        <v>402</v>
       </c>
       <c r="I84" s="14" t="s">
-        <v>419</v>
-      </c>
-      <c r="J84" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="K84" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="L84" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="M84" s="14"/>
+        <v>398</v>
+      </c>
+      <c r="J84" s="26" t="s">
+        <v>235</v>
+      </c>
+      <c r="K84" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="L84" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="M84" s="14" t="s">
+        <v>403</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85" s="12" t="s">
-        <v>424</v>
+        <v>404</v>
       </c>
       <c r="B85" s="18" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="C85" s="14" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="D85" s="14" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="E85" s="14" t="s">
-        <v>425</v>
+        <v>405</v>
       </c>
       <c r="F85" s="14" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="G85" s="14" t="s">
         <v>19</v>
       </c>
       <c r="H85" s="7" t="s">
-        <v>426</v>
+        <v>406</v>
       </c>
       <c r="I85" s="14" t="s">
-        <v>427</v>
-      </c>
-      <c r="J85" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="K85" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="L85" s="20">
+        <v>407</v>
+      </c>
+      <c r="J85" s="26" t="s">
+        <v>235</v>
+      </c>
+      <c r="K85" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="L85" s="22">
         <v>1.0</v>
       </c>
       <c r="M85" s="14" t="s">
-        <v>428</v>
+        <v>403</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="12" t="s">
-        <v>429</v>
+        <v>408</v>
       </c>
       <c r="B86" s="18" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="C86" s="14" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="D86" s="14" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="E86" s="14" t="s">
-        <v>430</v>
+        <v>409</v>
       </c>
       <c r="F86" s="14" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="G86" s="14" t="s">
         <v>19</v>
       </c>
       <c r="H86" s="7" t="s">
-        <v>431</v>
+        <v>410</v>
       </c>
       <c r="I86" s="14" t="s">
-        <v>432</v>
-      </c>
-      <c r="J86" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="K86" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="L86" s="20">
+        <v>411</v>
+      </c>
+      <c r="J86" s="26" t="s">
+        <v>235</v>
+      </c>
+      <c r="K86" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="L86" s="22">
         <v>1.0</v>
       </c>
       <c r="M86" s="14" t="s">
-        <v>433</v>
+        <v>412</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="12" t="s">
-        <v>434</v>
+        <v>413</v>
       </c>
       <c r="B87" s="18" t="s">
-        <v>435</v>
+        <v>414</v>
       </c>
       <c r="C87" s="14" t="s">
         <v>15</v>
@@ -6298,37 +6252,37 @@
         <v>16</v>
       </c>
       <c r="E87" s="14" t="s">
-        <v>436</v>
+        <v>415</v>
       </c>
       <c r="F87" s="14" t="s">
-        <v>266</v>
+        <v>235</v>
       </c>
       <c r="G87" s="14" t="s">
-        <v>437</v>
+        <v>416</v>
       </c>
       <c r="H87" s="7" t="s">
-        <v>438</v>
+        <v>417</v>
       </c>
       <c r="I87" s="19">
         <v>0.0416</v>
       </c>
-      <c r="J87" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="K87" s="21"/>
-      <c r="L87" s="20">
+      <c r="J87" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="K87" s="23"/>
+      <c r="L87" s="22">
         <v>1.0</v>
       </c>
       <c r="M87" s="14" t="s">
-        <v>439</v>
+        <v>418</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="12" t="s">
-        <v>440</v>
+        <v>419</v>
       </c>
       <c r="B88" s="18" t="s">
-        <v>435</v>
+        <v>414</v>
       </c>
       <c r="C88" s="14" t="s">
         <v>15</v>
@@ -6337,37 +6291,37 @@
         <v>16</v>
       </c>
       <c r="E88" s="14" t="s">
-        <v>441</v>
+        <v>420</v>
       </c>
       <c r="F88" s="14" t="s">
-        <v>266</v>
+        <v>235</v>
       </c>
       <c r="G88" s="14" t="s">
-        <v>442</v>
+        <v>421</v>
       </c>
       <c r="H88" s="7" t="s">
-        <v>443</v>
+        <v>422</v>
       </c>
       <c r="I88" s="19">
         <v>0.023</v>
       </c>
-      <c r="J88" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="K88" s="21"/>
-      <c r="L88" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="M88" s="14" t="s">
-        <v>444</v>
+      <c r="J88" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="K88" s="23"/>
+      <c r="L88" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="M88" s="24" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="12" t="s">
-        <v>445</v>
+        <v>423</v>
       </c>
       <c r="B89" s="18" t="s">
-        <v>435</v>
+        <v>414</v>
       </c>
       <c r="C89" s="14" t="s">
         <v>15</v>
@@ -6376,37 +6330,37 @@
         <v>16</v>
       </c>
       <c r="E89" s="14" t="s">
-        <v>446</v>
+        <v>424</v>
       </c>
       <c r="F89" s="14" t="s">
-        <v>266</v>
+        <v>235</v>
       </c>
       <c r="G89" s="14" t="s">
-        <v>447</v>
+        <v>425</v>
       </c>
       <c r="H89" s="7" t="s">
-        <v>448</v>
+        <v>426</v>
       </c>
       <c r="I89" s="15">
         <v>0.2</v>
       </c>
-      <c r="J89" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="K89" s="21"/>
-      <c r="L89" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="M89" s="14" t="s">
-        <v>449</v>
+      <c r="J89" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="K89" s="23"/>
+      <c r="L89" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="M89" s="24" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="12" t="s">
-        <v>450</v>
+        <v>427</v>
       </c>
       <c r="B90" s="18" t="s">
-        <v>435</v>
+        <v>414</v>
       </c>
       <c r="C90" s="14" t="s">
         <v>15</v>
@@ -6415,37 +6369,37 @@
         <v>16</v>
       </c>
       <c r="E90" s="14" t="s">
-        <v>451</v>
+        <v>428</v>
       </c>
       <c r="F90" s="14" t="s">
-        <v>266</v>
+        <v>235</v>
       </c>
       <c r="G90" s="14" t="s">
-        <v>452</v>
+        <v>429</v>
       </c>
       <c r="H90" s="7" t="s">
-        <v>453</v>
+        <v>430</v>
       </c>
       <c r="I90" s="19">
         <v>0.068</v>
       </c>
-      <c r="J90" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="K90" s="21"/>
-      <c r="L90" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="M90" s="14" t="s">
-        <v>454</v>
+      <c r="J90" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="K90" s="23"/>
+      <c r="L90" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="M90" s="24" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="12" t="s">
-        <v>455</v>
+        <v>431</v>
       </c>
       <c r="B91" s="18" t="s">
-        <v>435</v>
+        <v>414</v>
       </c>
       <c r="C91" s="14" t="s">
         <v>15</v>
@@ -6454,37 +6408,37 @@
         <v>16</v>
       </c>
       <c r="E91" s="14" t="s">
-        <v>456</v>
+        <v>432</v>
       </c>
       <c r="F91" s="14" t="s">
-        <v>266</v>
+        <v>235</v>
       </c>
       <c r="G91" s="14" t="s">
-        <v>457</v>
+        <v>433</v>
       </c>
       <c r="H91" s="7" t="s">
-        <v>458</v>
+        <v>434</v>
       </c>
       <c r="I91" s="15">
         <v>0.09</v>
       </c>
-      <c r="J91" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="K91" s="21"/>
-      <c r="L91" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="M91" s="14" t="s">
-        <v>459</v>
+      <c r="J91" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="K91" s="23"/>
+      <c r="L91" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="M91" s="24" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="12" t="s">
-        <v>460</v>
+        <v>435</v>
       </c>
       <c r="B92" s="18" t="s">
-        <v>435</v>
+        <v>414</v>
       </c>
       <c r="C92" s="14" t="s">
         <v>90</v>
@@ -6493,37 +6447,37 @@
         <v>16</v>
       </c>
       <c r="E92" s="14" t="s">
-        <v>461</v>
+        <v>436</v>
       </c>
       <c r="F92" s="14" t="s">
-        <v>266</v>
+        <v>235</v>
       </c>
       <c r="G92" s="14" t="s">
-        <v>462</v>
+        <v>437</v>
       </c>
       <c r="H92" s="7" t="s">
-        <v>463</v>
+        <v>438</v>
       </c>
       <c r="I92" s="15">
         <v>70.08</v>
       </c>
-      <c r="J92" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="K92" s="21"/>
-      <c r="L92" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="M92" s="25" t="s">
-        <v>464</v>
+      <c r="J92" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="K92" s="23"/>
+      <c r="L92" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="M92" s="31" t="s">
+        <v>439</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="12" t="s">
-        <v>465</v>
+        <v>440</v>
       </c>
       <c r="B93" s="18" t="s">
-        <v>435</v>
+        <v>414</v>
       </c>
       <c r="C93" s="14" t="s">
         <v>90</v>
@@ -6532,37 +6486,37 @@
         <v>16</v>
       </c>
       <c r="E93" s="14" t="s">
-        <v>466</v>
+        <v>441</v>
       </c>
       <c r="F93" s="14" t="s">
-        <v>266</v>
+        <v>235</v>
       </c>
       <c r="G93" s="14" t="s">
-        <v>467</v>
+        <v>442</v>
       </c>
       <c r="H93" s="7" t="s">
-        <v>468</v>
+        <v>443</v>
       </c>
       <c r="I93" s="19">
         <v>35.0</v>
       </c>
-      <c r="J93" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="K93" s="21"/>
-      <c r="L93" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="M93" s="25" t="s">
-        <v>469</v>
+      <c r="J93" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="K93" s="23"/>
+      <c r="L93" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="M93" s="32" t="s">
+        <v>444</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="12" t="s">
-        <v>470</v>
+        <v>445</v>
       </c>
       <c r="B94" s="18" t="s">
-        <v>435</v>
+        <v>414</v>
       </c>
       <c r="C94" s="14" t="s">
         <v>90</v>
@@ -6571,37 +6525,37 @@
         <v>16</v>
       </c>
       <c r="E94" s="14" t="s">
-        <v>471</v>
+        <v>446</v>
       </c>
       <c r="F94" s="14" t="s">
-        <v>266</v>
+        <v>235</v>
       </c>
       <c r="G94" s="14" t="s">
-        <v>472</v>
+        <v>447</v>
       </c>
       <c r="H94" s="7" t="s">
-        <v>473</v>
+        <v>448</v>
       </c>
       <c r="I94" s="15">
         <v>2.3</v>
       </c>
-      <c r="J94" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="K94" s="21"/>
-      <c r="L94" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="M94" s="25" t="s">
-        <v>474</v>
+      <c r="J94" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="K94" s="23"/>
+      <c r="L94" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="M94" s="31" t="s">
+        <v>449</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="12" t="s">
-        <v>475</v>
+        <v>450</v>
       </c>
       <c r="B95" s="18" t="s">
-        <v>435</v>
+        <v>414</v>
       </c>
       <c r="C95" s="14" t="s">
         <v>90</v>
@@ -6610,37 +6564,37 @@
         <v>16</v>
       </c>
       <c r="E95" s="14" t="s">
-        <v>476</v>
+        <v>451</v>
       </c>
       <c r="F95" s="14" t="s">
-        <v>266</v>
+        <v>235</v>
       </c>
       <c r="G95" s="14" t="s">
-        <v>477</v>
+        <v>452</v>
       </c>
       <c r="H95" s="7" t="s">
-        <v>478</v>
-      </c>
-      <c r="I95" s="26">
+        <v>453</v>
+      </c>
+      <c r="I95" s="33">
         <v>0.14</v>
       </c>
-      <c r="J95" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="K95" s="21"/>
-      <c r="L95" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="M95" s="25" t="s">
-        <v>479</v>
+      <c r="J95" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="K95" s="23"/>
+      <c r="L95" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="M95" s="31" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="12" t="s">
-        <v>480</v>
+        <v>454</v>
       </c>
       <c r="B96" s="18" t="s">
-        <v>435</v>
+        <v>414</v>
       </c>
       <c r="C96" s="14" t="s">
         <v>90</v>
@@ -6649,37 +6603,37 @@
         <v>16</v>
       </c>
       <c r="E96" s="14" t="s">
-        <v>481</v>
+        <v>455</v>
       </c>
       <c r="F96" s="14" t="s">
-        <v>266</v>
+        <v>235</v>
       </c>
       <c r="G96" s="14" t="s">
-        <v>482</v>
+        <v>456</v>
       </c>
       <c r="H96" s="7" t="s">
-        <v>483</v>
+        <v>457</v>
       </c>
       <c r="I96" s="15">
         <v>4.4</v>
       </c>
-      <c r="J96" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="K96" s="21"/>
-      <c r="L96" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="M96" s="25" t="s">
-        <v>484</v>
+      <c r="J96" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="K96" s="23"/>
+      <c r="L96" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="M96" s="31" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="12" t="s">
-        <v>485</v>
+        <v>458</v>
       </c>
       <c r="B97" s="18" t="s">
-        <v>435</v>
+        <v>414</v>
       </c>
       <c r="C97" s="14" t="s">
         <v>90</v>
@@ -6688,216 +6642,217 @@
         <v>16</v>
       </c>
       <c r="E97" s="14" t="s">
-        <v>486</v>
+        <v>459</v>
       </c>
       <c r="F97" s="14" t="s">
-        <v>266</v>
+        <v>235</v>
       </c>
       <c r="G97" s="14" t="s">
-        <v>487</v>
-      </c>
-      <c r="H97" s="7" t="s">
-        <v>488</v>
-      </c>
-      <c r="I97" s="26">
+        <v>460</v>
+      </c>
+      <c r="H97" s="34" t="s">
+        <v>461</v>
+      </c>
+      <c r="I97" s="33">
         <v>18.25</v>
       </c>
-      <c r="J97" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="K97" s="21"/>
-      <c r="L97" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="M97" s="25" t="s">
-        <v>489</v>
+      <c r="J97" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="K97" s="23"/>
+      <c r="L97" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="M97" s="31" t="s">
+        <v>462</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="12" t="s">
-        <v>490</v>
+        <v>463</v>
       </c>
       <c r="B98" s="18" t="s">
-        <v>435</v>
+        <v>414</v>
       </c>
       <c r="C98" s="14" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="D98" s="14" t="s">
         <v>16</v>
       </c>
       <c r="E98" s="14" t="s">
-        <v>491</v>
+        <v>464</v>
       </c>
       <c r="F98" s="14" t="s">
-        <v>266</v>
+        <v>235</v>
       </c>
       <c r="G98" s="14" t="s">
-        <v>492</v>
-      </c>
-      <c r="H98" s="7" t="s">
-        <v>493</v>
+        <v>465</v>
+      </c>
+      <c r="H98" s="35" t="s">
+        <v>466</v>
       </c>
       <c r="I98" s="27" t="s">
-        <v>494</v>
-      </c>
-      <c r="J98" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="K98" s="21"/>
-      <c r="L98" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="M98" s="25" t="s">
-        <v>495</v>
+        <v>467</v>
+      </c>
+      <c r="J98" s="23">
+        <v>1.0</v>
+      </c>
+      <c r="K98" s="23"/>
+      <c r="L98" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="M98" s="31" t="s">
+        <v>468</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="12" t="s">
-        <v>496</v>
+        <v>469</v>
       </c>
       <c r="B99" s="18" t="s">
-        <v>435</v>
+        <v>414</v>
       </c>
       <c r="C99" s="14" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="D99" s="14" t="s">
         <v>16</v>
       </c>
       <c r="E99" s="14" t="s">
-        <v>497</v>
+        <v>470</v>
       </c>
       <c r="F99" s="14" t="s">
-        <v>266</v>
+        <v>235</v>
       </c>
       <c r="G99" s="14" t="s">
-        <v>498</v>
+        <v>471</v>
       </c>
       <c r="H99" s="7" t="s">
-        <v>499</v>
+        <v>472</v>
       </c>
       <c r="I99" s="27">
         <v>407.34</v>
       </c>
-      <c r="J99" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="K99" s="21"/>
-      <c r="L99" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="M99" s="25" t="s">
-        <v>500</v>
+      <c r="J99" s="30">
+        <v>0.0</v>
+      </c>
+      <c r="K99" s="23"/>
+      <c r="L99" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="M99" s="31" t="s">
+        <v>473</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="12" t="s">
-        <v>501</v>
+        <v>474</v>
       </c>
       <c r="B100" s="18" t="s">
-        <v>435</v>
+        <v>414</v>
       </c>
       <c r="C100" s="14" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="D100" s="14" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="E100" s="14" t="s">
-        <v>502</v>
+        <v>475</v>
       </c>
       <c r="F100" s="14" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="G100" s="14" t="s">
         <v>19</v>
       </c>
       <c r="H100" s="7" t="s">
-        <v>503</v>
+        <v>476</v>
       </c>
       <c r="I100" s="19" t="s">
-        <v>504</v>
-      </c>
-      <c r="J100" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="K100" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="L100" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="M100" s="28" t="s">
-        <v>505</v>
+        <v>477</v>
+      </c>
+      <c r="J100" s="26" t="s">
+        <v>235</v>
+      </c>
+      <c r="K100" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="L100" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="M100" s="36" t="s">
+        <v>478</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="12" t="s">
-        <v>506</v>
+        <v>479</v>
       </c>
       <c r="B101" s="18" t="s">
-        <v>435</v>
+        <v>414</v>
       </c>
       <c r="C101" s="14" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="D101" s="14" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="E101" s="14" t="s">
-        <v>507</v>
+        <v>480</v>
       </c>
       <c r="F101" s="14" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="G101" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="H101" s="29" t="s">
-        <v>508</v>
-      </c>
-      <c r="I101" s="30" t="s">
-        <v>509</v>
-      </c>
-      <c r="J101" s="31">
-        <v>1.0</v>
-      </c>
-      <c r="K101" s="31">
-        <v>1.0</v>
-      </c>
-      <c r="L101" s="31">
-        <v>1.0</v>
-      </c>
-      <c r="M101" s="28" t="s">
-        <v>510</v>
+      <c r="H101" s="37" t="s">
+        <v>481</v>
+      </c>
+      <c r="I101" s="38" t="s">
+        <v>482</v>
+      </c>
+      <c r="J101" s="39" t="s">
+        <v>235</v>
+      </c>
+      <c r="K101" s="40">
+        <v>1.0</v>
+      </c>
+      <c r="L101" s="40">
+        <v>1.0</v>
+      </c>
+      <c r="M101" s="36" t="s">
+        <v>483</v>
       </c>
     </row>
     <row r="102">
-      <c r="A102" s="32"/>
-      <c r="B102" s="32"/>
-      <c r="C102" s="32"/>
-      <c r="D102" s="32"/>
-      <c r="E102" s="32"/>
-      <c r="F102" s="32"/>
-      <c r="G102" s="32"/>
-      <c r="H102" s="33" t="s">
-        <v>511</v>
-      </c>
-      <c r="I102" s="34"/>
-      <c r="J102" s="35">
-        <f t="shared" ref="J102:L102" si="1">SUM(J2:J101)</f>
-        <v>94</v>
-      </c>
-      <c r="K102" s="35">
-        <f t="shared" si="1"/>
-        <v>12</v>
-      </c>
-      <c r="L102" s="35">
-        <f t="shared" si="1"/>
-        <v>97</v>
-      </c>
-      <c r="M102" s="32"/>
+      <c r="A102" s="41"/>
+      <c r="B102" s="41"/>
+      <c r="C102" s="41"/>
+      <c r="D102" s="41"/>
+      <c r="E102" s="41"/>
+      <c r="F102" s="41"/>
+      <c r="G102" s="41"/>
+      <c r="H102" s="42" t="s">
+        <v>484</v>
+      </c>
+      <c r="I102" s="43"/>
+      <c r="J102" s="44">
+        <f>SUM(J2:J101)/(100-COUNTIF(J1:J101,"N/A"))
+</f>
+        <v>0.9090909091</v>
+      </c>
+      <c r="K102" s="44">
+        <f>SUM(K2:K101)/12</f>
+        <v>1</v>
+      </c>
+      <c r="L102" s="44">
+        <f>SUM(L2:L101)/100</f>
+        <v>1</v>
+      </c>
+      <c r="M102" s="41"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>